<commit_message>
updated sulfonamide and tetracycline antibiotics
</commit_message>
<xml_diff>
--- a/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
+++ b/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmol/Git/MAxO/src/patterns/data/todo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{599D1813-0D19-CA45-B48C-572E31EF91DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D28A65-65B9-654A-9E09-9120CA9E43F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10820" yWindow="720" windowWidth="27640" windowHeight="16940" xr2:uid="{23FC4AE2-4209-3D4D-8A45-DA0E48B55CFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="149">
   <si>
     <t>defined_class</t>
   </si>
@@ -129,6 +129,24 @@
     <t>topical anaesthtic</t>
   </si>
   <si>
+    <t>anti-infective agent</t>
+  </si>
+  <si>
+    <t>MAXO_0000325</t>
+  </si>
+  <si>
+    <t>MAXO_0000174</t>
+  </si>
+  <si>
+    <t>MAXO_0001021</t>
+  </si>
+  <si>
+    <t>MAXO_0000061</t>
+  </si>
+  <si>
+    <t>MAXO_0000227</t>
+  </si>
+  <si>
     <t>MAXO_0000058</t>
   </si>
   <si>
@@ -283,13 +301,184 @@
   </si>
   <si>
     <t>anti-estrogen drug</t>
+  </si>
+  <si>
+    <t>MAXO_0000169</t>
+  </si>
+  <si>
+    <t>anti-inflammatory agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI_35472</t>
+  </si>
+  <si>
+    <t>anti-inflammatory drug</t>
+  </si>
+  <si>
+    <t>MAXO_0000221</t>
+  </si>
+  <si>
+    <t>nsaid therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000173</t>
+  </si>
+  <si>
+    <t>CHEBI_50919</t>
+  </si>
+  <si>
+    <t>antiemetic therapy</t>
+  </si>
+  <si>
+    <t>antiemetic</t>
+  </si>
+  <si>
+    <t>CHEBI_66956</t>
+  </si>
+  <si>
+    <t>antidyskinesia agent</t>
+  </si>
+  <si>
+    <t>antidyskinesia agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000636</t>
+  </si>
+  <si>
+    <t>anti-infective agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI_35441</t>
+  </si>
+  <si>
+    <t>anti-fungal agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI_86327</t>
+  </si>
+  <si>
+    <t>anti-fungal agent</t>
+  </si>
+  <si>
+    <t>CHEBI_36043</t>
+  </si>
+  <si>
+    <t>antimicrobial agent therapy</t>
+  </si>
+  <si>
+    <t>antibacterial agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI_36047</t>
+  </si>
+  <si>
+    <t>CHEBI_64912</t>
+  </si>
+  <si>
+    <t>antimycobacterial agent</t>
+  </si>
+  <si>
+    <t>antimycobacterial agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000228</t>
+  </si>
+  <si>
+    <t>CHEBI_33231</t>
+  </si>
+  <si>
+    <t>antitubercular agent</t>
+  </si>
+  <si>
+    <t>antitubercular agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000229</t>
+  </si>
+  <si>
+    <t>CHEBI_35816</t>
+  </si>
+  <si>
+    <t>leprostatic drug</t>
+  </si>
+  <si>
+    <t>leprostatic agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000432</t>
+  </si>
+  <si>
+    <t>beta-lactam antibacterial agent therapy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEBI:27933 </t>
+  </si>
+  <si>
+    <t>beta-lactam antibiotic</t>
+  </si>
+  <si>
+    <t>MAXO_0000197</t>
+  </si>
+  <si>
+    <t>cephalosporin agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:23066</t>
+  </si>
+  <si>
+    <t>cephalosporin antibiotic</t>
+  </si>
+  <si>
+    <t>CHEBI:17334</t>
+  </si>
+  <si>
+    <t>penicillin</t>
+  </si>
+  <si>
+    <t>penicillin agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000198</t>
+  </si>
+  <si>
+    <t>MAXO_0000200</t>
+  </si>
+  <si>
+    <t>macrolide antibacterial agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:25105</t>
+  </si>
+  <si>
+    <t>macrolide</t>
+  </si>
+  <si>
+    <t>CHEBI:86324</t>
+  </si>
+  <si>
+    <t>quiniolone antibioctic</t>
+  </si>
+  <si>
+    <t>MAXO_0000201</t>
+  </si>
+  <si>
+    <t>quinolone antibacterial agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:87228</t>
+  </si>
+  <si>
+    <t>sulfonamide antibiotic</t>
+  </si>
+  <si>
+    <t>MAXO_0000202</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -321,6 +510,13 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -342,12 +538,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D020C68-606D-2948-9201-7F6682425891}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -711,16 +908,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -728,7 +925,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -742,7 +939,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>22</v>
@@ -756,7 +953,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>29</v>
@@ -770,7 +967,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
@@ -781,10 +978,10 @@
     </row>
     <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>25</v>
@@ -795,10 +992,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>27</v>
@@ -809,10 +1006,10 @@
     </row>
     <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>32</v>
@@ -826,7 +1023,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -840,7 +1037,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>12</v>
@@ -851,150 +1048,368 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="C24" s="4"/>
+      <c r="A24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="C25" s="4"/>
+      <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="C26" s="4"/>
+      <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="C27" s="4"/>
+      <c r="A27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="C28" s="4"/>
+      <c r="A28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="C29" s="4"/>
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish anti-viral therapy update. #176
</commit_message>
<xml_diff>
--- a/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
+++ b/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmol/Git/MAxO/src/patterns/data/todo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEFCC40-F05D-484F-A7D7-42252129A430}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805342F1-0E78-D348-A508-B131AD678610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10820" yWindow="720" windowWidth="27640" windowHeight="16940" xr2:uid="{23FC4AE2-4209-3D4D-8A45-DA0E48B55CFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="190">
   <si>
     <t>defined_class</t>
   </si>
@@ -569,12 +569,60 @@
   <si>
     <t>HIV protease inhibitor therapy</t>
   </si>
+  <si>
+    <t>CHEBI:64952</t>
+  </si>
+  <si>
+    <t>anti-HSV agent</t>
+  </si>
+  <si>
+    <t>MAXO_0000637</t>
+  </si>
+  <si>
+    <t>anti-HSV agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:64953</t>
+  </si>
+  <si>
+    <t>anti-HSV-1 agent</t>
+  </si>
+  <si>
+    <t>MAXO_0000638</t>
+  </si>
+  <si>
+    <t>anti-HSV-1 agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:64954</t>
+  </si>
+  <si>
+    <t>anti-HSV-2 agent</t>
+  </si>
+  <si>
+    <t>MAXO_0000639</t>
+  </si>
+  <si>
+    <t>anti-HSV-2 agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000220</t>
+  </si>
+  <si>
+    <t>CHEBI:24261</t>
+  </si>
+  <si>
+    <t>glucocorticoid</t>
+  </si>
+  <si>
+    <t>glucocorticicoid agent therapy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -625,6 +673,12 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -646,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -654,6 +708,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D020C68-606D-2948-9201-7F6682425891}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1578,13 +1633,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>168</v>
@@ -1602,6 +1657,62 @@
       </c>
       <c r="D43" s="1" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsoleted enzyme replacements and modifier agent therapy added other anti-inflammatory terms. #176
</commit_message>
<xml_diff>
--- a/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
+++ b/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmol/Git/MAxO/src/patterns/data/todo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805342F1-0E78-D348-A508-B131AD678610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D919069-7F29-F647-8AEE-28F19A613ECF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10820" yWindow="720" windowWidth="27640" windowHeight="16940" xr2:uid="{23FC4AE2-4209-3D4D-8A45-DA0E48B55CFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="198">
   <si>
     <t>defined_class</t>
   </si>
@@ -617,12 +617,36 @@
   <si>
     <t>glucocorticicoid agent therapy</t>
   </si>
+  <si>
+    <t>MAXO_0000640</t>
+  </si>
+  <si>
+    <t>corticosteroid</t>
+  </si>
+  <si>
+    <t>corticosteroid therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:50858</t>
+  </si>
+  <si>
+    <t>MAXO_0000642</t>
+  </si>
+  <si>
+    <t>emetic therapy</t>
+  </si>
+  <si>
+    <t>CHEBI_149552</t>
+  </si>
+  <si>
+    <t>emetic</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -679,6 +703,13 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -700,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -709,6 +740,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D020C68-606D-2948-9201-7F6682425891}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1715,6 +1747,34 @@
         <v>188</v>
       </c>
     </row>
+    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update enzyme modifying therapy
</commit_message>
<xml_diff>
--- a/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
+++ b/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmol/Git/MAxO/src/patterns/data/todo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D919069-7F29-F647-8AEE-28F19A613ECF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096130BD-FE35-0349-9745-1B2868B84A58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10820" yWindow="720" windowWidth="27640" windowHeight="16940" xr2:uid="{23FC4AE2-4209-3D4D-8A45-DA0E48B55CFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="214">
   <si>
     <t>defined_class</t>
   </si>
@@ -641,12 +641,60 @@
   <si>
     <t>emetic</t>
   </si>
+  <si>
+    <t>CHEBI_35845</t>
+  </si>
+  <si>
+    <t>gout suppressant</t>
+  </si>
+  <si>
+    <t>antigout therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000164</t>
+  </si>
+  <si>
+    <t>CHEBI_35842</t>
+  </si>
+  <si>
+    <t>antirheumatic drug</t>
+  </si>
+  <si>
+    <t>MAXO_0000643</t>
+  </si>
+  <si>
+    <t>antirheumatic agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:38462</t>
+  </si>
+  <si>
+    <t>EC 3.1.1.7 (acetylcholinesterase) inhibitor</t>
+  </si>
+  <si>
+    <t>acetylcholinesterase inhibitor</t>
+  </si>
+  <si>
+    <t>MAXO_0000645</t>
+  </si>
+  <si>
+    <t>MAXO_0000210</t>
+  </si>
+  <si>
+    <t>cholinesteriase inhibitor</t>
+  </si>
+  <si>
+    <t>CHEBI:37733</t>
+  </si>
+  <si>
+    <t>EC 3.1.1.8 (cholinesterase) inhibitor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -710,6 +758,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF007C82"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -731,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -741,6 +795,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D020C68-606D-2948-9201-7F6682425891}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1775,6 +1830,62 @@
         <v>197</v>
       </c>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="23" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="23" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update antineoplastics, antispasticity, etc.
</commit_message>
<xml_diff>
--- a/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
+++ b/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmol/Git/MAxO/src/patterns/data/todo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096130BD-FE35-0349-9745-1B2868B84A58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA408EC-D907-304A-9A97-D7CF1417425C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10820" yWindow="720" windowWidth="27640" windowHeight="16940" xr2:uid="{23FC4AE2-4209-3D4D-8A45-DA0E48B55CFA}"/>
+    <workbookView xWindow="10760" yWindow="720" windowWidth="27640" windowHeight="16940" xr2:uid="{23FC4AE2-4209-3D4D-8A45-DA0E48B55CFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="218">
   <si>
     <t>defined_class</t>
   </si>
@@ -688,6 +688,18 @@
   </si>
   <si>
     <t>EC 3.1.1.8 (cholinesterase) inhibitor</t>
+  </si>
+  <si>
+    <t>MAXO_0000062</t>
+  </si>
+  <si>
+    <t>antineoplastic agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:35610</t>
+  </si>
+  <si>
+    <t>antineoplastic agent</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D020C68-606D-2948-9201-7F6682425891}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1886,6 +1898,20 @@
         <v>213</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update glucose regulator therapies.
</commit_message>
<xml_diff>
--- a/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
+++ b/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmol/Git/MAxO/src/patterns/data/todo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA408EC-D907-304A-9A97-D7CF1417425C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBC0CD4-5C89-C748-8112-C18CEB5E1038}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="720" windowWidth="27640" windowHeight="16940" xr2:uid="{23FC4AE2-4209-3D4D-8A45-DA0E48B55CFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="244">
   <si>
     <t>defined_class</t>
   </si>
@@ -295,9 +295,6 @@
   </si>
   <si>
     <t>MAXO_0000635</t>
-  </si>
-  <si>
-    <t>anti-estrogent agent therapy</t>
   </si>
   <si>
     <t>anti-estrogen drug</t>
@@ -701,12 +698,93 @@
   <si>
     <t>antineoplastic agent</t>
   </si>
+  <si>
+    <t>anti-estrogen agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000230</t>
+  </si>
+  <si>
+    <t>akylating agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:22333</t>
+  </si>
+  <si>
+    <t>akylating agent</t>
+  </si>
+  <si>
+    <t>CHEBI:23924</t>
+  </si>
+  <si>
+    <t>enzyme inhibitor</t>
+  </si>
+  <si>
+    <t>enzyme inhibitor agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000648</t>
+  </si>
+  <si>
+    <t>CHEBI:50790</t>
+  </si>
+  <si>
+    <t>EC 1.14.14.14 (aromatase) inhibitor</t>
+  </si>
+  <si>
+    <t>MAXO_0000234</t>
+  </si>
+  <si>
+    <t>aromatase inhibitor agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000237</t>
+  </si>
+  <si>
+    <t>retinoid agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:51371</t>
+  </si>
+  <si>
+    <t>muscle relaxant</t>
+  </si>
+  <si>
+    <t>MAXO_0000245</t>
+  </si>
+  <si>
+    <t>antspasticity agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:35526</t>
+  </si>
+  <si>
+    <t>hypoglycemic agent</t>
+  </si>
+  <si>
+    <t>hypoglycemic agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000572</t>
+  </si>
+  <si>
+    <t>MAXO_0000649</t>
+  </si>
+  <si>
+    <t>hyperglycemic agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:76916</t>
+  </si>
+  <si>
+    <t>hyper glycemic agent</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -776,6 +854,12 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -797,7 +881,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -808,6 +892,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1122,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D020C68-606D-2948-9201-7F6682425891}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1426,69 +1511,69 @@
         <v>89</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>90</v>
+        <v>217</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -1496,10 +1581,10 @@
         <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>34</v>
@@ -1511,13 +1596,13 @@
         <v>36</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -1525,13 +1610,13 @@
         <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -1539,13 +1624,13 @@
         <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -1553,363 +1638,455 @@
         <v>39</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="D32" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="C36" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="C37" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="C40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="C41" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="C44" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="C45" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="C46" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>190</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="C51" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="23" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C52" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="9" t="s">
         <v>206</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="23" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>217</v>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D57" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating cardiovascular agent therapy
</commit_message>
<xml_diff>
--- a/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
+++ b/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmol/Git/MAxO/src/patterns/data/todo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBC0CD4-5C89-C748-8112-C18CEB5E1038}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539D62D1-0621-1847-906F-3CC44901F862}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="720" windowWidth="27640" windowHeight="16940" xr2:uid="{23FC4AE2-4209-3D4D-8A45-DA0E48B55CFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="252">
   <si>
     <t>defined_class</t>
   </si>
@@ -778,6 +778,30 @@
   </si>
   <si>
     <t>hyper glycemic agent</t>
+  </si>
+  <si>
+    <t>CHEBI:35554</t>
+  </si>
+  <si>
+    <t>cardiovascular drug</t>
+  </si>
+  <si>
+    <t>cardiovascular agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000181</t>
+  </si>
+  <si>
+    <t>MAXO_0000185</t>
+  </si>
+  <si>
+    <t>antiarrythmic agent tehrapy</t>
+  </si>
+  <si>
+    <t>CHEBI:38070</t>
+  </si>
+  <si>
+    <t>anti-arrhythmia drug</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D020C68-606D-2948-9201-7F6682425891}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2089,6 +2113,34 @@
         <v>243</v>
       </c>
     </row>
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update calcium channel modulator therapy
</commit_message>
<xml_diff>
--- a/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
+++ b/src/patterns/data/todo/pharmacotherapy_chemicalsubstance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmol/Git/MAxO/src/patterns/data/todo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539D62D1-0621-1847-906F-3CC44901F862}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31A4995-4D4B-AC4C-8740-B923A1F6ECFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="720" windowWidth="27640" windowHeight="16940" xr2:uid="{23FC4AE2-4209-3D4D-8A45-DA0E48B55CFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="291">
   <si>
     <t>defined_class</t>
   </si>
@@ -795,13 +795,130 @@
     <t>MAXO_0000185</t>
   </si>
   <si>
-    <t>antiarrythmic agent tehrapy</t>
-  </si>
-  <si>
     <t>CHEBI:38070</t>
   </si>
   <si>
     <t>anti-arrhythmia drug</t>
+  </si>
+  <si>
+    <t>MAXO_0000650</t>
+  </si>
+  <si>
+    <t>antiatherogenic agent therapy</t>
+  </si>
+  <si>
+    <t>antiarrythmic agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:50855</t>
+  </si>
+  <si>
+    <t>antiatherogenic agent</t>
+  </si>
+  <si>
+    <t>CHEBI:145947</t>
+  </si>
+  <si>
+    <t>antiaterosclerotic agent</t>
+  </si>
+  <si>
+    <t>antiatherosclerotic agent therapy</t>
+  </si>
+  <si>
+    <t>MAXO_0000651</t>
+  </si>
+  <si>
+    <t>MAXO_0001025</t>
+  </si>
+  <si>
+    <t>adrenergic agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:37962</t>
+  </si>
+  <si>
+    <t>adrenergic agent</t>
+  </si>
+  <si>
+    <t>MAXO_0000182</t>
+  </si>
+  <si>
+    <t>alpha adrenergic agent therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:48539</t>
+  </si>
+  <si>
+    <t>alpha-adrenergic drug</t>
+  </si>
+  <si>
+    <t>MAXO_0000183</t>
+  </si>
+  <si>
+    <t>MAXO_0000184</t>
+  </si>
+  <si>
+    <t>alpha adrenergic agonist therapy</t>
+  </si>
+  <si>
+    <t>alpha adrenergic antagonist therapy</t>
+  </si>
+  <si>
+    <t>CHEBI:48540</t>
+  </si>
+  <si>
+    <t>CHEBI:37890</t>
+  </si>
+  <si>
+    <t>MAXO_0000186</t>
+  </si>
+  <si>
+    <t>MAXO_0001026</t>
+  </si>
+  <si>
+    <t>CHEBI:35522</t>
+  </si>
+  <si>
+    <t>beta-adrenergic agonist therapy</t>
+  </si>
+  <si>
+    <t>beta adrenergic agent therapy</t>
+  </si>
+  <si>
+    <t>alpha-adrenergic agonist drug</t>
+  </si>
+  <si>
+    <t>alpha-adrenergic antagonist drug</t>
+  </si>
+  <si>
+    <t>beta-adrenergic agent thearpy</t>
+  </si>
+  <si>
+    <t>beta-adrenergic agonist drug</t>
+  </si>
+  <si>
+    <t>MAXO_0000187</t>
+  </si>
+  <si>
+    <t>CHEBI:35530</t>
+  </si>
+  <si>
+    <t>beta-adrenergic antagonist therapy</t>
+  </si>
+  <si>
+    <t>beta-adrenergic antagonist drug</t>
+  </si>
+  <si>
+    <t>CHEBI:38215</t>
+  </si>
+  <si>
+    <t>MAXO_0000434</t>
+  </si>
+  <si>
+    <t>calcium channel blocking agent</t>
+  </si>
+  <si>
+    <t>calcium channel blocker</t>
   </si>
 </sst>
 </file>
@@ -1231,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D020C68-606D-2948-9201-7F6682425891}">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2132,13 +2249,153 @@
         <v>248</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C63" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="D63" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D63" s="1" t="s">
+    </row>
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>251</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>